<commit_message>
CCDB-325: Enabling defualt values in DataLoader.
</commit_message>
<xml_diff>
--- a/conf-core/src/test/resources/dataloader/device-type-fail-update.xlsx
+++ b/conf-core/src/test/resources/dataloader/device-type-fail-update.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="40">
   <si>
     <t>NAME</t>
   </si>
@@ -41,9 +41,6 @@
     <t>BPM1</t>
   </si>
   <si>
-    <t>ACENPOS</t>
-  </si>
-  <si>
     <t>Date</t>
   </si>
   <si>
@@ -141,9 +138,6 @@
   </si>
   <si>
     <t>accept</t>
-  </si>
-  <si>
-    <t>APERTURE</t>
   </si>
   <si>
     <t>Help</t>
@@ -240,11 +234,11 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -526,7 +520,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F358"/>
+  <dimension ref="A1:F356"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -541,126 +535,126 @@
   <sheetData>
     <row r="1" spans="1:6" ht="21.95" customHeight="1">
       <c r="A1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
         <v>6</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>8</v>
-      </c>
       <c r="E1">
-        <f>SUMPRODUCT((B13:B65469&lt;&gt;"")/COUNTIF(B13:B65469,B13:B65469&amp;""))</f>
-        <v>3.0000000000000004</v>
+        <f>SUMPRODUCT((B13:B65467&lt;&gt;"")/COUNTIF(B13:B65467,B13:B65467&amp;""))</f>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="21.95" customHeight="1">
       <c r="A2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>11</v>
-      </c>
       <c r="E2">
-        <f>SUMPRODUCT((E11:E65516&lt;&gt;"")/COUNTIF(E11:E65516,E11:E65516&amp;""))</f>
-        <v>4</v>
+        <f>SUMPRODUCT((E11:E65514&lt;&gt;"")/COUNTIF(E11:E65514,E11:E65514&amp;""))</f>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="21.95" customHeight="1">
       <c r="A3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
         <v>12</v>
       </c>
-      <c r="B3" t="s">
+      <c r="D3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="E3">
-        <f>COUNTIF(A11:A65466,"CREATE DEVICE TYPE")+COUNTIF(A11:A65466,"CREATE PROPERTY")</f>
+        <f>COUNTIF(A11:A65464,"CREATE DEVICE TYPE")+COUNTIF(A11:A65464,"CREATE PROPERTY")</f>
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="21.95" customHeight="1">
       <c r="A4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
         <v>15</v>
       </c>
-      <c r="B4" t="s">
+      <c r="D4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="E4">
-        <f>COUNTIF(A11:A65466,"UPDATE DEVICE TYPE")+COUNTIF(A11:A65466,"UPDATE PROPERTY")</f>
-        <v>9</v>
+        <f>COUNTIF(A11:A65464,"UPDATE DEVICE TYPE")+COUNTIF(A11:A65464,"UPDATE PROPERTY")</f>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="21.95" customHeight="1">
       <c r="A5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" t="s">
         <v>18</v>
       </c>
-      <c r="B5" t="s">
+      <c r="D5" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>20</v>
-      </c>
       <c r="E5">
-        <f>COUNTIF(A11:A65466,"DELETE DEVICE TYPE")+COUNTIF(A11:A65466,"DELETE PROPERTY")</f>
+        <f>COUNTIF(A11:A65464,"DELETE DEVICE TYPE")+COUNTIF(A11:A65464,"DELETE PROPERTY")</f>
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="21.95" customHeight="1">
       <c r="A6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" t="s">
         <v>21</v>
       </c>
-      <c r="B6" t="s">
-        <v>22</v>
-      </c>
     </row>
     <row r="7" spans="1:6" ht="21.95" customHeight="1">
-      <c r="A7" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>41</v>
+      <c r="A7" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="21.75" customHeight="1"/>
     <row r="9" spans="1:6" ht="21.95" customHeight="1">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="C9" s="7"/>
+      <c r="D9" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
     </row>
     <row r="10" spans="1:6" ht="21.95" customHeight="1">
-      <c r="A10" s="5"/>
+      <c r="A10" s="7"/>
       <c r="B10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C10" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" s="4" t="s">
         <v>26</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>27</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="21.95" customHeight="1">
@@ -668,10 +662,10 @@
         <v>1</v>
       </c>
       <c r="B11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" t="s">
         <v>29</v>
-      </c>
-      <c r="C11" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="21.95" customHeight="1">
@@ -679,10 +673,10 @@
         <v>1</v>
       </c>
       <c r="B12" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" t="s">
         <v>31</v>
-      </c>
-      <c r="C12" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="21.75" customHeight="1">
@@ -690,10 +684,10 @@
         <v>1</v>
       </c>
       <c r="B13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" t="s">
         <v>33</v>
-      </c>
-      <c r="C13" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="21.75" customHeight="1">
@@ -704,10 +698,10 @@
         <v>3</v>
       </c>
       <c r="E14" t="s">
+        <v>34</v>
+      </c>
+      <c r="F14" t="s">
         <v>35</v>
-      </c>
-      <c r="F14" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="21.75" customHeight="1">
@@ -718,84 +712,68 @@
         <v>3</v>
       </c>
       <c r="E15" t="s">
+        <v>36</v>
+      </c>
+      <c r="F15" t="s">
         <v>37</v>
-      </c>
-      <c r="F15" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="21.75" customHeight="1">
       <c r="A16" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B16" t="s">
-        <v>4</v>
-      </c>
-      <c r="E16" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="21.75" customHeight="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="21.75" customHeight="1">
       <c r="A17" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B17" t="s">
         <v>4</v>
       </c>
-      <c r="E17" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="21.75" customHeight="1">
-      <c r="A18" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="21.75" customHeight="1">
-      <c r="A19" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B19" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="2"/>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="2"/>
+    </row>
+    <row r="20" spans="1:2">
       <c r="A20" s="2"/>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:2">
       <c r="A21" s="2"/>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:2">
       <c r="A22" s="2"/>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:2">
       <c r="A23" s="2"/>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:2">
       <c r="A24" s="2"/>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:2">
       <c r="A25" s="2"/>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:2">
       <c r="A26" s="2"/>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:2">
       <c r="A27" s="2"/>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:2">
       <c r="A28" s="2"/>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:2">
       <c r="A29" s="2"/>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:2">
       <c r="A30" s="2"/>
     </row>
-    <row r="31" spans="1:5">
+    <row r="31" spans="1:2">
       <c r="A31" s="2"/>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:2">
       <c r="A32" s="2"/>
     </row>
     <row r="33" spans="1:1">
@@ -1769,12 +1747,6 @@
     </row>
     <row r="356" spans="1:1">
       <c r="A356" s="2"/>
-    </row>
-    <row r="357" spans="1:1">
-      <c r="A357" s="2"/>
-    </row>
-    <row r="358" spans="1:1">
-      <c r="A358" s="2"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0" selectUnlockedCells="1"/>

</xml_diff>